<commit_message>
Listado de tipos de movimientos, modificacion de reporte, validacion y envio de datos
</commit_message>
<xml_diff>
--- a/Payroll/Content/REPORTES/MOVIMIENTOS/MOVIMIENTOS_E4_A2020_P20_T3.xlsx
+++ b/Payroll/Content/REPORTES/MOVIMIENTOS/MOVIMIENTOS_E4_A2020_P20_T3.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>Empresa</t>
   </si>
@@ -120,6 +120,15 @@
   </si>
   <si>
     <t xml:space="preserve">Dic  7 2020 12:35PM</t>
+  </si>
+  <si>
+    <t>Cambio de puesto</t>
+  </si>
+  <si>
+    <t>9077.97</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dic  8 2020  1:31PM</t>
   </si>
 </sst>
 </file>
@@ -174,7 +183,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="xr">
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -408,6 +417,44 @@
         <v>20</v>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" s="0">
+        <v>4</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="0">
+        <v>20</v>
+      </c>
+      <c r="F7" s="0">
+        <v>2020</v>
+      </c>
+      <c r="G7" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="H7" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="I7" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="J7" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="K7" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="L7" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <headerFooter/>
 </worksheet>

</xml_diff>